<commit_message>
additional weekly and monthly reports with filtered
</commit_message>
<xml_diff>
--- a/server/public/templates/reports_2023-10-01_2023-10-31.xlsx
+++ b/server/public/templates/reports_2023-10-01_2023-10-31.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Fullname</t>
   </si>
@@ -19,19 +19,16 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>ContactNo</t>
-  </si>
-  <si>
     <t>Karl Borromeo</t>
   </si>
   <si>
-    <t>09123456789</t>
-  </si>
-  <si>
     <t>Mary Grace Galllardo</t>
   </si>
   <si>
     <t>Kryzz Andig</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
@@ -408,57 +405,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="3" width="25" customWidth="1"/>
+    <col min="1" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>1000</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>2000</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
       </c>
       <c r="B4">
         <v>4000</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
       <c r="B5">
         <v>7000</v>
       </c>

</xml_diff>